<commit_message>
CMM018-M : perfect version
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
@@ -129,7 +129,7 @@
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">未登録一覧!$A$1:$G$52</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">未登録一覧!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">未登録一覧!$1:$3</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[9]!PrintDaicho</definedName>
     <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[9]!QuitDaicho</definedName>
@@ -348,10 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm"/>
-  </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,21 +437,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
@@ -576,7 +558,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3">
       <alignment vertical="center"/>
@@ -587,28 +569,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -44509,10 +44479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -44534,55 +44504,40 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="8"/>
+    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:7">
+      <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G4" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D2:E3"/>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.393700787" right="0.393700787" top="0.59055118100000004" bottom="0.59055118110236204" header="0.56496062999999996" footer="0.31496062992126"/>
@@ -44591,8 +44546,5 @@
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;9【会社】日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,Bold"&amp;14承認ルート未登録社員一覧&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;D&amp;T
 &amp;Nページ</oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="52" max="6" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CMM018-M: fix template of screen L and paging of screen M
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
@@ -44481,7 +44481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -44544,7 +44544,7 @@
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0">
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;9【会社】日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,Bold"&amp;14承認ルート未登録社員一覧&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;D&amp;T
-&amp;Nページ</oddHeader>
+&amp;Pページ</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CMM018_2次: Chỉnh templace + ...
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/承認ルート未登録の社員のEXCEL出力.xlsx
@@ -342,25 +342,24 @@
   </si>
   <si>
     <t>所属職場名</t>
-    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -368,7 +367,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -376,7 +375,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -389,7 +388,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -417,7 +416,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -450,6 +449,12 @@
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -559,7 +564,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3">
       <alignment vertical="center"/>
@@ -570,9 +575,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,6 +583,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -44508,61 +44525,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="1.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="2.75" style="1"/>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="1.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="2.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>